<commit_message>
restructure packages for modularization, establishing base class concept
</commit_message>
<xml_diff>
--- a/docs/ColorScale-ALL.xlsx
+++ b/docs/ColorScale-ALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\myFiles\Git\Catatumbo\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C059D459-A9C5-4C01-AB3A-FB77F41BBC3E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E065967-0BCA-4AE2-8F4A-AC627FC2D5A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{6254D5CB-A900-47F5-A6E3-719C72A36DDA}"/>
+    <workbookView xWindow="1464" yWindow="36" windowWidth="17304" windowHeight="12468" activeTab="1" xr2:uid="{6254D5CB-A900-47F5-A6E3-719C72A36DDA}"/>
   </bookViews>
   <sheets>
     <sheet name="forecast" sheetId="1" r:id="rId1"/>
@@ -1252,6 +1252,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1261,7 +1262,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5987,7 +5987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA4B77B-4853-4A74-8659-0A438A7CF41A}">
   <dimension ref="B1:R118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:R13"/>
     </sheetView>
   </sheetViews>
@@ -6018,18 +6018,18 @@
       <c r="P1" s="127"/>
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="G2" s="138" t="s">
+      <c r="G2" s="139" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
+      <c r="H2" s="139"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="139"/>
+      <c r="K2" s="139"/>
+      <c r="L2" s="139"/>
+      <c r="M2" s="139"/>
+      <c r="N2" s="139"/>
+      <c r="O2" s="139"/>
+      <c r="P2" s="139"/>
       <c r="Q2" s="125"/>
     </row>
     <row r="3" spans="2:18" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
@@ -6048,7 +6048,7 @@
       <c r="E4" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="139" t="s">
+      <c r="G4" s="140" t="s">
         <v>56</v>
       </c>
       <c r="H4" s="103">
@@ -6097,7 +6097,7 @@
         <f>"+2.5%"</f>
         <v>+2.5%</v>
       </c>
-      <c r="G5" s="139"/>
+      <c r="G5" s="140"/>
       <c r="H5" s="103">
         <v>1.2</v>
       </c>
@@ -6140,7 +6140,7 @@
         <f>"+1.2%"</f>
         <v>+1.2%</v>
       </c>
-      <c r="G6" s="139"/>
+      <c r="G6" s="140"/>
       <c r="H6" s="103">
         <v>0.3</v>
       </c>
@@ -6186,7 +6186,7 @@
         <f>"+0.3%"</f>
         <v>+0.3%</v>
       </c>
-      <c r="G7" s="139"/>
+      <c r="G7" s="140"/>
       <c r="H7" s="137">
         <v>0</v>
       </c>
@@ -6232,7 +6232,7 @@
         <f>"+0%"</f>
         <v>+0%</v>
       </c>
-      <c r="G8" s="139"/>
+      <c r="G8" s="140"/>
       <c r="H8" s="103">
         <v>-0.3</v>
       </c>
@@ -6280,7 +6280,7 @@
         <f>"-0.3%"</f>
         <v>-0.3%</v>
       </c>
-      <c r="G9" s="139"/>
+      <c r="G9" s="140"/>
       <c r="H9" s="103">
         <v>-1.2</v>
       </c>
@@ -6330,7 +6330,7 @@
         <f>"-1.2%"</f>
         <v>-1.2%</v>
       </c>
-      <c r="G10" s="139"/>
+      <c r="G10" s="140"/>
       <c r="H10" s="103">
         <v>-2.5</v>
       </c>
@@ -6491,7 +6491,7 @@
       <c r="I22" s="103" t="s">
         <v>70</v>
       </c>
-      <c r="K22" s="141" t="s">
+      <c r="K22" s="138" t="s">
         <v>68</v>
       </c>
       <c r="N22" s="130" t="s">
@@ -6504,7 +6504,7 @@
       <c r="I23" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="K23" s="141" t="s">
+      <c r="K23" s="138" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6514,18 +6514,18 @@
       </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="140" t="s">
+      <c r="B26" s="141" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="140"/>
-      <c r="D26" s="140" t="s">
+      <c r="C26" s="141"/>
+      <c r="D26" s="141" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140" t="s">
+      <c r="E26" s="141"/>
+      <c r="F26" s="141" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="140"/>
+      <c r="G26" s="141"/>
     </row>
     <row r="27" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B27" s="130"/>
@@ -7968,7 +7968,7 @@
         <v>-1.9</v>
       </c>
       <c r="D92" s="102">
-        <f t="shared" ref="D92:D123" si="7">$D$27/2+ROUND(ABS($D$27/(1+EXP(0.8*C92))-$D$27/2),0)</f>
+        <f t="shared" ref="D92:D118" si="7">$D$27/2+ROUND(ABS($D$27/(1+EXP(0.8*C92))-$D$27/2),0)</f>
         <v>208</v>
       </c>
       <c r="E92" s="103">

</xml_diff>